<commit_message>
feat: read weather excel
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C\fast-weather-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818BE58E-A9AB-4792-9E61-29BA79855305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212DCCAB-1E69-4E66-87F6-7C1C21806BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="4272" windowWidth="23040" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17388" yWindow="-9984" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
feat: write weather excel
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C\fast-weather-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{212DCCAB-1E69-4E66-87F6-7C1C21806BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68631495-CFA4-45CA-A054-FA5B85BE8951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17388" yWindow="-9984" windowWidth="17496" windowHeight="30336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15468" yWindow="-8064" windowWidth="12876" windowHeight="22284" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>EXCEL_FILE_NAME</t>
   </si>
@@ -28,13 +28,16 @@
     <t>EXCEL_SHEET_NAME</t>
   </si>
   <si>
-    <t>DATE_COLUMN_EXCEL_INDEX</t>
-  </si>
-  <si>
     <t>Sheet1</t>
   </si>
   <si>
     <t>weather_data</t>
+  </si>
+  <si>
+    <t>DATE_COLUMN_LETTER</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -436,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -447,13 +450,13 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>